<commit_message>
Corrected SMD sizes, updated BOM and placement.
</commit_message>
<xml_diff>
--- a/hardware/ps2/ps2usb-BOM.xlsx
+++ b/hardware/ps2/ps2usb-BOM.xlsx
@@ -9,7 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Enclosure" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
-  <si>
-    <t xml:space="preserve">Designators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quant</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+  <si>
+    <t xml:space="preserve">Designator</t>
   </si>
   <si>
     <t xml:space="preserve">Manufacturer</t>
@@ -38,10 +34,10 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Package</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
+    <t xml:space="preserve">Footprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JLCPCB Part #</t>
   </si>
   <si>
     <t xml:space="preserve">C1,C2,C5,C6,C7</t>
@@ -59,6 +55,9 @@
     <t xml:space="preserve">SMD 0603</t>
   </si>
   <si>
+    <t xml:space="preserve">C342962</t>
+  </si>
+  <si>
     <t xml:space="preserve">C3,C4</t>
   </si>
   <si>
@@ -71,13 +70,16 @@
     <t xml:space="preserve">Cap, 0603, MLCC, 10pF, 50v, C0G</t>
   </si>
   <si>
+    <t xml:space="preserve">C1634</t>
+  </si>
+  <si>
     <t xml:space="preserve">D1</t>
   </si>
   <si>
-    <t xml:space="preserve">Shenzhen Tuozhan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P4-1204RGBWS2-1.5T-A</t>
+    <t xml:space="preserve">Harvatek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B3173BGR-20C0001Q3U1930</t>
   </si>
   <si>
     <t xml:space="preserve">LED, RGB, Common Anode</t>
@@ -86,7 +88,7 @@
     <t xml:space="preserve">SMD</t>
   </si>
   <si>
-    <t xml:space="preserve">Alt: Harvatek B3173BGR-20C0001Q3U1930</t>
+    <t xml:space="preserve">C2827295</t>
   </si>
   <si>
     <t xml:space="preserve">RN1,RN2</t>
@@ -101,6 +103,9 @@
     <t xml:space="preserve">SMD 4x0603</t>
   </si>
   <si>
+    <t xml:space="preserve">C110021</t>
+  </si>
+  <si>
     <t xml:space="preserve">RN3</t>
   </si>
   <si>
@@ -110,6 +115,9 @@
     <t xml:space="preserve">Res Array, 4x0603, 120R</t>
   </si>
   <si>
+    <t xml:space="preserve">C136835</t>
+  </si>
+  <si>
     <t xml:space="preserve">J1,J2</t>
   </si>
   <si>
@@ -125,7 +133,7 @@
     <t xml:space="preserve">Through-Hole</t>
   </si>
   <si>
-    <t xml:space="preserve">TH</t>
+    <t xml:space="preserve">C7428703</t>
   </si>
   <si>
     <t xml:space="preserve">J3</t>
@@ -140,15 +148,15 @@
     <t xml:space="preserve">Conn, USB, 2.0, Type-A, Dual</t>
   </si>
   <si>
-    <t xml:space="preserve">J5</t>
+    <t xml:space="preserve">C456021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J4</t>
   </si>
   <si>
     <t xml:space="preserve">DO NOT POPULATE</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
     <t xml:space="preserve">U1</t>
   </si>
   <si>
@@ -164,19 +172,22 @@
     <t xml:space="preserve">SMD QFP48</t>
   </si>
   <si>
+    <t xml:space="preserve">C150548</t>
+  </si>
+  <si>
     <t xml:space="preserve">S1</t>
   </si>
   <si>
-    <t xml:space="preserve">Shenzhen Kinghelm Elec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KH-6X6X9H-ZJ</t>
+    <t xml:space="preserve">CUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS11-674-95-BK-160-RA-D</t>
   </si>
   <si>
     <t xml:space="preserve">Switch, Tactile, Right Angle, 9mm Actuator Length</t>
   </si>
   <si>
-    <t xml:space="preserve">Alt: CUI TS11-674-95-BK-160-RA-D</t>
+    <t xml:space="preserve">C7074168</t>
   </si>
   <si>
     <t xml:space="preserve">F1</t>
@@ -194,6 +205,9 @@
     <t xml:space="preserve">SMD 1206</t>
   </si>
   <si>
+    <t xml:space="preserve">C883126</t>
+  </si>
+  <si>
     <t xml:space="preserve">Y1</t>
   </si>
   <si>
@@ -209,28 +223,7 @@
     <t xml:space="preserve">SMD 3225</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Hammond </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">1455D601xx</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">60.0 x 42.5 x 23.0 mm Aluminum Enclosure</t>
+    <t xml:space="preserve">C9002</t>
   </si>
 </sst>
 </file>
@@ -240,7 +233,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -272,6 +265,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -282,7 +283,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -327,7 +328,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -340,11 +341,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -471,7 +484,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -480,20 +493,19 @@
   <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="41.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -505,350 +517,245 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="4" t="n">
-        <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="str">
-        <f aca="false">LEFT(F2,3)</f>
-        <v>SMD</v>
-      </c>
-      <c r="H2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="n">
-        <v>2</v>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="4" t="str">
-        <f aca="false">LEFT(F3,3)</f>
-        <v>SMD</v>
-      </c>
-      <c r="H3" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="4" t="n">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="4" t="str">
-        <f aca="false">LEFT(F4,3)</f>
-        <v>SMD</v>
-      </c>
-      <c r="H4" s="4" t="s">
         <v>21</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="4" t="n">
-        <v>2</v>
+        <v>23</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="4" t="str">
-        <f aca="false">LEFT(F5,3)</f>
-        <v>SMD</v>
-      </c>
-      <c r="H5" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="4" t="str">
-        <f aca="false">LEFT(F6,3)</f>
-        <v>SMD</v>
-      </c>
-      <c r="H6" s="4"/>
+      <c r="F6" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="4" t="n">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="4" t="n">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="4"/>
+      <c r="F8" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="4" t="n">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="4"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="4" t="n">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="4" t="str">
-        <f aca="false">LEFT(F10,3)</f>
-        <v>SMD</v>
-      </c>
-      <c r="H10" s="4"/>
+        <v>49</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>51</v>
+        <v>36</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="4" t="n">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="4" t="str">
-        <f aca="false">LEFT(F12,3)</f>
-        <v>SMD</v>
-      </c>
-      <c r="H12" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="4" t="n">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" s="4" t="str">
-        <f aca="false">LEFT(F13,3)</f>
-        <v>SMD</v>
-      </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16377" style="0" width="11.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated recommended length of button
8mm actuator length instead of 9.5mm.  JLCPCB part number not updated due to lack of availability.
</commit_message>
<xml_diff>
--- a/hardware/ps2/ps2usb-BOM.xlsx
+++ b/hardware/ps2/ps2usb-BOM.xlsx
@@ -181,10 +181,10 @@
     <t xml:space="preserve">CUI</t>
   </si>
   <si>
-    <t xml:space="preserve">TS11-674-95-BK-160-RA-D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switch, Tactile, Right Angle, 9mm Actuator Length</t>
+    <t xml:space="preserve">TS11-674-80-BK-160-RA-D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch, Tactile, Right Angle, 8mm Actuator Length</t>
   </si>
   <si>
     <t xml:space="preserve">C7074168</t>
@@ -233,7 +233,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -279,12 +279,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -328,7 +322,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -341,7 +335,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -349,15 +343,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -497,8 +483,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="41.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -531,13 +517,13 @@
       <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -551,13 +537,13 @@
       <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -565,19 +551,19 @@
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -591,13 +577,13 @@
       <c r="C5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -611,13 +597,13 @@
       <c r="C6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -631,13 +617,13 @@
       <c r="C7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -651,13 +637,13 @@
       <c r="C8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -694,7 +680,7 @@
       <c r="E10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -705,7 +691,7 @@
       <c r="B11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -714,7 +700,7 @@
       <c r="E11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -734,7 +720,7 @@
       <c r="E12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -754,7 +740,7 @@
       <c r="E13" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>